<commit_message>
add Excel export of matches of KuersatClassifier
</commit_message>
<xml_diff>
--- a/test/PDFLib/SampleSizesComplete.xlsx
+++ b/test/PDFLib/SampleSizesComplete.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ground Truth" sheetId="1" r:id="rId1"/>
@@ -19371,7 +19371,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -21320,7 +21319,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21364,7 +21363,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9293311" cy="6011047"/>
+    <xdr:ext cx="9317935" cy="6032500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -71692,7 +71691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>

</xml_diff>